<commit_message>
SD-77548 - Problem with visible some atomics for KPI SSD aviaballity
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/KPI_Atomic_Names_Update.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/KPI_Atomic_Names_Update.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
   <si>
     <t xml:space="preserve">KPI Set</t>
   </si>
@@ -128,14 +128,27 @@
   </si>
   <si>
     <t xml:space="preserve">Coca-Cola - 0.25L Slim/0.33L Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PoS 2019 - MT Conv Big - REG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice Tea Shelf: Top Shelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice Tea Shelf: Fuze Berry-Hibiscus- 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice Tea Shelf: Fuze Berry-Hibiscus - 1L</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -234,7 +247,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -257,6 +270,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -276,19 +297,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.3622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.9387755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.8010204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="91.9285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="85.8571428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="90.8469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -558,6 +578,30 @@
       <c r="E16" s="0" t="str">
         <f aca="false">CONCATENATE("UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='",D16,"', a.description='",D16,"', a.display_text='",D16,"'  WHERE s.name='",A16,"' AND k.display_text='",B16,"' AND a.name='",C16,"';")</f>
         <v>UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='Coca-Cola - 0.25L Slim/0.33L Glass', a.description='Coca-Cola - 0.25L Slim/0.33L Glass', a.display_text='Coca-Cola - 0.25L Slim/0.33L Glass'  WHERE s.name='PoS 2019 - IC Canteen - EDU' AND k.display_text='SSD Availability' AND a.name='Coca-Cola - 0.25L Slim/Coca-Cola - 0.33L Glass';</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="0" t="str">
+        <f aca="false">CONCATENATE("UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='",D18,"', a.description='",D18,"', a.display_text='",D18,"'  WHERE s.name='",A18,"' AND k.display_text='",B18,"' AND a.name='",C18,"';")</f>
+        <v>UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='Ice Tea Shelf: Fuze Berry-Hibiscus - 1L', a.description='Ice Tea Shelf: Fuze Berry-Hibiscus - 1L', a.display_text='Ice Tea Shelf: Fuze Berry-Hibiscus - 1L'  WHERE s.name='PoS 2019 - MT Conv Big - REG' AND k.display_text='Ice Tea Shelf: Top Shelf' AND a.name='Ice Tea Shelf: Fuze Berry-Hibiscus- 1L';</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PROS-9213 - CCRU - rename KPI and add EAN code for some new Products
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/KPI_Atomic_Names_Update.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/KPI_Atomic_Names_Update.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="52">
   <si>
     <t xml:space="preserve">KPI Set</t>
   </si>
@@ -140,6 +140,42 @@
   </si>
   <si>
     <t xml:space="preserve">Ice Tea Shelf: Fuze Berry-Hibiscus - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PoS 2019 - IC Petroleum - CAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEW SKU 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pulpy - Guava-Passion Fruit - 0.45L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEW SKU 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pulpy - Watermelon-Strawberry - 0.45L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PoS 2019 - MT Conv Big - CAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice (JNSD) Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEW SKU 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PoS 2019 - MT Hypermarket - CAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PoS 2019 - MT Hypermarket - REG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PoS 2019 - MT Supermarket - CAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PoS 2019 - MT Supermarket - REG</t>
   </si>
 </sst>
 </file>
@@ -186,7 +222,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,6 +239,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
   </fills>
@@ -247,7 +289,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -280,6 +322,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -289,6 +335,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF00B050"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -297,18 +403,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="85.8571428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="90.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="84.9081632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="89.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -602,6 +709,258 @@
       <c r="E18" s="0" t="str">
         <f aca="false">CONCATENATE("UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='",D18,"', a.description='",D18,"', a.display_text='",D18,"'  WHERE s.name='",A18,"' AND k.display_text='",B18,"' AND a.name='",C18,"';")</f>
         <v>UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='Ice Tea Shelf: Fuze Berry-Hibiscus - 1L', a.description='Ice Tea Shelf: Fuze Berry-Hibiscus - 1L', a.display_text='Ice Tea Shelf: Fuze Berry-Hibiscus - 1L'  WHERE s.name='PoS 2019 - MT Conv Big - REG' AND k.display_text='Ice Tea Shelf: Top Shelf' AND a.name='Ice Tea Shelf: Fuze Berry-Hibiscus- 1L';</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="0" t="str">
+        <f aca="false">CONCATENATE("UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='",D20,"', a.description='",D20,"', a.display_text='",D20,"'  WHERE s.name='",A20,"' AND k.display_text='",B20,"' AND a.name='",C20,"';")</f>
+        <v>UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='Pulpy - Guava-Passion Fruit - 0.45L', a.description='Pulpy - Guava-Passion Fruit - 0.45L', a.display_text='Pulpy - Guava-Passion Fruit - 0.45L'  WHERE s.name='PoS 2019 - IC Petroleum - CAP' AND k.display_text='Juice Availability' AND a.name='NEW SKU 7';</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="0" t="str">
+        <f aca="false">CONCATENATE("UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='",D21,"', a.description='",D21,"', a.display_text='",D21,"'  WHERE s.name='",A21,"' AND k.display_text='",B21,"' AND a.name='",C21,"';")</f>
+        <v>UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='Pulpy - Watermelon-Strawberry - 0.45L', a.description='Pulpy - Watermelon-Strawberry - 0.45L', a.display_text='Pulpy - Watermelon-Strawberry - 0.45L'  WHERE s.name='PoS 2019 - IC Petroleum - CAP' AND k.display_text='Juice Availability' AND a.name='NEW SKU 8';</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="0" t="str">
+        <f aca="false">CONCATENATE("UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='",D22,"', a.description='",D22,"', a.display_text='",D22,"'  WHERE s.name='",A22,"' AND k.display_text='",B22,"' AND a.name='",C22,"';")</f>
+        <v>UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='Pulpy - Guava-Passion Fruit - 0.45L', a.description='Pulpy - Guava-Passion Fruit - 0.45L', a.display_text='Pulpy - Guava-Passion Fruit - 0.45L'  WHERE s.name='PoS 2019 - IC Petroleum - CAP' AND k.display_text='Juice Availability' AND a.name='NEW SKU 7';</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="0" t="str">
+        <f aca="false">CONCATENATE("UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='",D23,"', a.description='",D23,"', a.display_text='",D23,"'  WHERE s.name='",A23,"' AND k.display_text='",B23,"' AND a.name='",C23,"';")</f>
+        <v>UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='Pulpy - Watermelon-Strawberry - 0.45L', a.description='Pulpy - Watermelon-Strawberry - 0.45L', a.display_text='Pulpy - Watermelon-Strawberry - 0.45L'  WHERE s.name='PoS 2019 - IC Petroleum - CAP' AND k.display_text='Juice Availability' AND a.name='NEW SKU 8';</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="0" t="str">
+        <f aca="false">CONCATENATE("UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='",D24,"', a.description='",D24,"', a.display_text='",D24,"'  WHERE s.name='",A24,"' AND k.display_text='",B24,"' AND a.name='",C24,"';")</f>
+        <v>UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='Pulpy - Guava-Passion Fruit - 0.45L', a.description='Pulpy - Guava-Passion Fruit - 0.45L', a.display_text='Pulpy - Guava-Passion Fruit - 0.45L'  WHERE s.name='PoS 2019 - MT Conv Big - CAP' AND k.display_text='Juice (JNSD) Availability' AND a.name='NEW SKU 6';</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="0" t="str">
+        <f aca="false">CONCATENATE("UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='",D25,"', a.description='",D25,"', a.display_text='",D25,"'  WHERE s.name='",A25,"' AND k.display_text='",B25,"' AND a.name='",C25,"';")</f>
+        <v>UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='Pulpy - Guava-Passion Fruit - 0.45L', a.description='Pulpy - Guava-Passion Fruit - 0.45L', a.display_text='Pulpy - Guava-Passion Fruit - 0.45L'  WHERE s.name='PoS 2019 - MT Conv Big - REG' AND k.display_text='Juice (JNSD) Availability' AND a.name='NEW SKU 6';</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="0" t="str">
+        <f aca="false">CONCATENATE("UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='",D26,"', a.description='",D26,"', a.display_text='",D26,"'  WHERE s.name='",A26,"' AND k.display_text='",B26,"' AND a.name='",C26,"';")</f>
+        <v>UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='Pulpy - Guava-Passion Fruit - 0.45L', a.description='Pulpy - Guava-Passion Fruit - 0.45L', a.display_text='Pulpy - Guava-Passion Fruit - 0.45L'  WHERE s.name='PoS 2019 - MT Hypermarket - CAP' AND k.display_text='Juice (JNSD) Availability' AND a.name='NEW SKU 6';</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="0" t="str">
+        <f aca="false">CONCATENATE("UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='",D27,"', a.description='",D27,"', a.display_text='",D27,"'  WHERE s.name='",A27,"' AND k.display_text='",B27,"' AND a.name='",C27,"';")</f>
+        <v>UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='Pulpy - Watermelon-Strawberry - 0.45L', a.description='Pulpy - Watermelon-Strawberry - 0.45L', a.display_text='Pulpy - Watermelon-Strawberry - 0.45L'  WHERE s.name='PoS 2019 - MT Hypermarket - CAP' AND k.display_text='Juice (JNSD) Availability' AND a.name='NEW SKU 8';</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" s="0" t="str">
+        <f aca="false">CONCATENATE("UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='",D28,"', a.description='",D28,"', a.display_text='",D28,"'  WHERE s.name='",A28,"' AND k.display_text='",B28,"' AND a.name='",C28,"';")</f>
+        <v>UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='Pulpy - Guava-Passion Fruit - 0.45L', a.description='Pulpy - Guava-Passion Fruit - 0.45L', a.display_text='Pulpy - Guava-Passion Fruit - 0.45L'  WHERE s.name='PoS 2019 - MT Hypermarket - REG' AND k.display_text='Juice (JNSD) Availability' AND a.name='NEW SKU 6';</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29" s="0" t="str">
+        <f aca="false">CONCATENATE("UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='",D29,"', a.description='",D29,"', a.display_text='",D29,"'  WHERE s.name='",A29,"' AND k.display_text='",B29,"' AND a.name='",C29,"';")</f>
+        <v>UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='Pulpy - Watermelon-Strawberry - 0.45L', a.description='Pulpy - Watermelon-Strawberry - 0.45L', a.display_text='Pulpy - Watermelon-Strawberry - 0.45L'  WHERE s.name='PoS 2019 - MT Hypermarket - REG' AND k.display_text='Juice (JNSD) Availability' AND a.name='NEW SKU 8';</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" s="0" t="str">
+        <f aca="false">CONCATENATE("UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='",D30,"', a.description='",D30,"', a.display_text='",D30,"'  WHERE s.name='",A30,"' AND k.display_text='",B30,"' AND a.name='",C30,"';")</f>
+        <v>UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='Pulpy - Guava-Passion Fruit - 0.45L', a.description='Pulpy - Guava-Passion Fruit - 0.45L', a.display_text='Pulpy - Guava-Passion Fruit - 0.45L'  WHERE s.name='PoS 2019 - MT Supermarket - CAP' AND k.display_text='Juice (JNSD) Availability' AND a.name='NEW SKU 6';</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="0" t="str">
+        <f aca="false">CONCATENATE("UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='",D31,"', a.description='",D31,"', a.display_text='",D31,"'  WHERE s.name='",A31,"' AND k.display_text='",B31,"' AND a.name='",C31,"';")</f>
+        <v>UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='Pulpy - Watermelon-Strawberry - 0.45L', a.description='Pulpy - Watermelon-Strawberry - 0.45L', a.display_text='Pulpy - Watermelon-Strawberry - 0.45L'  WHERE s.name='PoS 2019 - MT Supermarket - CAP' AND k.display_text='Juice (JNSD) Availability' AND a.name='NEW SKU 8';</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="0" t="str">
+        <f aca="false">CONCATENATE("UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='",D32,"', a.description='",D32,"', a.display_text='",D32,"'  WHERE s.name='",A32,"' AND k.display_text='",B32,"' AND a.name='",C32,"';")</f>
+        <v>UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='Pulpy - Guava-Passion Fruit - 0.45L', a.description='Pulpy - Guava-Passion Fruit - 0.45L', a.display_text='Pulpy - Guava-Passion Fruit - 0.45L'  WHERE s.name='PoS 2019 - MT Supermarket - REG' AND k.display_text='Juice (JNSD) Availability' AND a.name='NEW SKU 6';</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33" s="0" t="str">
+        <f aca="false">CONCATENATE("UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='",D33,"', a.description='",D33,"', a.display_text='",D33,"'  WHERE s.name='",A33,"' AND k.display_text='",B33,"' AND a.name='",C33,"';")</f>
+        <v>UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='Pulpy - Watermelon-Strawberry - 0.45L', a.description='Pulpy - Watermelon-Strawberry - 0.45L', a.display_text='Pulpy - Watermelon-Strawberry - 0.45L'  WHERE s.name='PoS 2019 - MT Supermarket - REG' AND k.display_text='Juice (JNSD) Availability' AND a.name='NEW SKU 8';</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PROS-10834 - CCRU - POS files update
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/KPI_Atomic_Names_Update.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/KPI_Atomic_Names_Update.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="81">
   <si>
     <t xml:space="preserve">KPI Set</t>
   </si>
@@ -239,6 +239,30 @@
   </si>
   <si>
     <t xml:space="preserve">Dobriy - Multifruit - 0.33L/Rich Orange 0.3L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice Display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice Display: Lead SKU Dobriy - Apple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice Display: Lead SKU Dobriy Apple/Multi 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PoS 2019 - FT - CAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Display: Lead SKU Coca-Cola - 1L/1.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Display: Lead SKU Coca-Cola - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PoS 2019 - FT - REG</t>
   </si>
 </sst>
 </file>
@@ -505,19 +529,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E45" activeCellId="0" sqref="E45:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="80.9948979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="85.7193877551021"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="80.0510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="84.7755102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1207,6 +1231,78 @@
       <c r="E43" s="0" t="str">
         <f aca="false">CONCATENATE("UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='",D43,"', a.description='",D43,"', a.display_text='",D43,"'  WHERE s.name='",A43,"' AND k.display_text='",B43,"' AND a.name='",C43,"';")</f>
         <v>UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='Dobriy - Multifruit - 0.33L/Rich Orange 0.3L', a.description='Dobriy - Multifruit - 0.33L/Rich Orange 0.3L', a.display_text='Dobriy - Multifruit - 0.33L/Rich Orange 0.3L'  WHERE s.name='PoS 2019 - IC FastFood' AND k.display_text='Juice Availability' AND a.name='Dobriy - Multifruit - 0.33L';</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E45" s="0" t="str">
+        <f aca="false">CONCATENATE("UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='",D45,"', a.description='",D45,"', a.display_text='",D45,"'  WHERE s.name='",A45,"' AND k.display_text='",B45,"' AND a.name='",C45,"';")</f>
+        <v>UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='Juice Display: Lead SKU Dobriy Apple/Multi 1L', a.description='Juice Display: Lead SKU Dobriy Apple/Multi 1L', a.display_text='Juice Display: Lead SKU Dobriy Apple/Multi 1L'  WHERE s.name='PoS 2019 - FT NS - CAP' AND k.display_text='Juice Display' AND a.name='Juice Display: Lead SKU Dobriy - Apple';</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E46" s="0" t="str">
+        <f aca="false">CONCATENATE("UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='",D46,"', a.description='",D46,"', a.display_text='",D46,"'  WHERE s.name='",A46,"' AND k.display_text='",B46,"' AND a.name='",C46,"';")</f>
+        <v>UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='Juice Display: Lead SKU Dobriy Apple/Multi 1L', a.description='Juice Display: Lead SKU Dobriy Apple/Multi 1L', a.display_text='Juice Display: Lead SKU Dobriy Apple/Multi 1L'  WHERE s.name='PoS 2019 - FT NS - REG' AND k.display_text='Juice Display' AND a.name='Juice Display: Lead SKU Dobriy - Apple';</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E47" s="0" t="str">
+        <f aca="false">CONCATENATE("UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='",D47,"', a.description='",D47,"', a.display_text='",D47,"'  WHERE s.name='",A47,"' AND k.display_text='",B47,"' AND a.name='",C47,"';")</f>
+        <v>UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='SSD Display: Lead SKU Coca-Cola - 1L', a.description='SSD Display: Lead SKU Coca-Cola - 1L', a.display_text='SSD Display: Lead SKU Coca-Cola - 1L'  WHERE s.name='PoS 2019 - FT - CAP' AND k.display_text='SSD Display' AND a.name='SSD Display: Lead SKU Coca-Cola - 1L/1.5L';</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E48" s="0" t="str">
+        <f aca="false">CONCATENATE("UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='",D48,"', a.description='",D48,"', a.display_text='",D48,"'  WHERE s.name='",A48,"' AND k.display_text='",B48,"' AND a.name='",C48,"';")</f>
+        <v>UPDATE `static`.atomic_kpi a JOIN `static`.kpi k ON k.pk=a.kpi_fk JOIN `static`.kpi_set s ON s.pk=k.kpi_set_fk   SET a.name='SSD Display: Lead SKU Coca-Cola - 1L', a.description='SSD Display: Lead SKU Coca-Cola - 1L', a.display_text='SSD Display: Lead SKU Coca-Cola - 1L'  WHERE s.name='PoS 2019 - FT - REG' AND k.display_text='SSD Display' AND a.name='SSD Display: Lead SKU Coca-Cola - 1L/1.5L';</v>
       </c>
     </row>
   </sheetData>

</xml_diff>